<commit_message>
fix import data master
data kube, data rutilahu, data sarling
</commit_message>
<xml_diff>
--- a/import_data_template/template_kube.xlsx
+++ b/import_data_template/template_kube.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kemensos\import_data_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79220DEF-6B92-4E48-BA69-79D2ED1E4A38}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D873E746-90F7-440D-BBE3-53F94A732082}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -504,11 +504,11 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -851,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BY364"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -891,10 +891,10 @@
       <c r="F1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="32"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="19" t="s">
         <v>10</v>
       </c>
@@ -918,7 +918,7 @@
       </c>
     </row>
     <row r="2" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -959,7 +959,7 @@
       <c r="O2" s="27"/>
     </row>
     <row r="3" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
+      <c r="A3" s="32"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="21"/>
@@ -990,7 +990,7 @@
       <c r="O3" s="27"/>
     </row>
     <row r="4" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="21"/>
@@ -1021,7 +1021,7 @@
       <c r="O4" s="27"/>
     </row>
     <row r="5" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="21"/>
@@ -1052,7 +1052,7 @@
       <c r="O5" s="27"/>
     </row>
     <row r="6" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="21"/>
@@ -1083,7 +1083,7 @@
       <c r="O6" s="27"/>
     </row>
     <row r="7" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="21"/>
@@ -1114,7 +1114,7 @@
       <c r="O7" s="27"/>
     </row>
     <row r="8" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="21"/>
@@ -1145,7 +1145,7 @@
       <c r="O8" s="27"/>
     </row>
     <row r="9" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="21"/>
@@ -1176,7 +1176,7 @@
       <c r="O9" s="27"/>
     </row>
     <row r="10" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="21"/>
@@ -1207,7 +1207,7 @@
       <c r="O10" s="27"/>
     </row>
     <row r="11" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="21"/>
@@ -1238,7 +1238,7 @@
       <c r="O11" s="27"/>
     </row>
     <row r="12" spans="1:77" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31">
+      <c r="A12" s="32">
         <v>2</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1279,7 +1279,7 @@
       <c r="O12" s="27"/>
     </row>
     <row r="13" spans="1:77" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="21"/>
@@ -1372,7 +1372,7 @@
       <c r="BY13" s="12"/>
     </row>
     <row r="14" spans="1:77" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="21"/>
@@ -1465,7 +1465,7 @@
       <c r="BY14" s="12"/>
     </row>
     <row r="15" spans="1:77" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="21"/>
@@ -1558,7 +1558,7 @@
       <c r="BY15" s="12"/>
     </row>
     <row r="16" spans="1:77" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="21"/>
@@ -1651,7 +1651,7 @@
       <c r="BY16" s="12"/>
     </row>
     <row r="17" spans="1:77" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="21"/>
@@ -1744,7 +1744,7 @@
       <c r="BY17" s="12"/>
     </row>
     <row r="18" spans="1:77" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="21"/>
@@ -1837,7 +1837,7 @@
       <c r="BY18" s="12"/>
     </row>
     <row r="19" spans="1:77" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="21"/>
@@ -1930,7 +1930,7 @@
       <c r="BY19" s="12"/>
     </row>
     <row r="20" spans="1:77" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="21"/>
@@ -2023,7 +2023,7 @@
       <c r="BY20" s="12"/>
     </row>
     <row r="21" spans="1:77" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="21"/>

</xml_diff>